<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@51f357645aed2293dd681ea7e33d6e3bb0cfbc74 🚀
</commit_message>
<xml_diff>
--- a/chat.xlsx
+++ b/chat.xlsx
@@ -1655,11 +1655,11 @@
       <c r="G13" s="47" t="inlineStr">
         <is>
           <t>Animation nationale:
-Paul Hurel
+Paul hurel
 Suivi scientifique:
 Yoann Bressan
 Sandrine Ruette
-Animation régionale:
+Animateur régional:
 Cédric Mondy</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@be8f1e35534e8a9ca4550cbbff5c81039e1eb978 🚀
</commit_message>
<xml_diff>
--- a/chat.xlsx
+++ b/chat.xlsx
@@ -1716,12 +1716,12 @@
           <t>Animation nationale:
 Paul HUREL
 Suivi scientifique:
+Maëlle TEYSSEIRE
 Yoann BRESSAN
-Sandrine RUETTE
 Animation régionale:
 Cédric MONDY
 Correspondants départementaux:
-PPC: Sylvain BERANGER
+PPC: 
 77: Anne-Gaëlle BLANC
 78-95: Amandine EVRARD
 91: Cyril KLEINPRINZ</t>
@@ -2525,7 +2525,7 @@
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="inlineStr">
         <is>
-          <t>Editée le 2024-07-24</t>
+          <t>Editée le 2024-12-09</t>
         </is>
       </c>
       <c r="B49" s="2"/>

</xml_diff>